<commit_message>
Update part list of power proto board
</commit_message>
<xml_diff>
--- a/Power_Board/WDY_Power_Board - MDP/WDY_Power_Board_Part_List.xlsx
+++ b/Power_Board/WDY_Power_Board - MDP/WDY_Power_Board_Part_List.xlsx
@@ -28,23 +28,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="74">
   <si>
     <t>Value</t>
   </si>
   <si>
-    <t>Package</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
     <t>2.2uF</t>
   </si>
   <si>
-    <t>C0603</t>
-  </si>
-  <si>
     <t>GRT188R61H225KE13D</t>
   </si>
   <si>
@@ -57,30 +51,18 @@
     <t>22uF</t>
   </si>
   <si>
-    <t>C0805</t>
-  </si>
-  <si>
     <t>STPS3L40UF</t>
   </si>
   <si>
-    <t>SMB</t>
-  </si>
-  <si>
     <t>MBRS140</t>
   </si>
   <si>
-    <t>DO-214AA</t>
-  </si>
-  <si>
     <t>MBRS140T3G</t>
   </si>
   <si>
     <t>FUSE3557L</t>
   </si>
   <si>
-    <t>3557-LITTLE</t>
-  </si>
-  <si>
     <t>22-05-7028-02</t>
   </si>
   <si>
@@ -90,33 +72,21 @@
     <t>10uH</t>
   </si>
   <si>
-    <t>WE-PD2_5848/5820</t>
-  </si>
-  <si>
     <t>15uH</t>
   </si>
   <si>
     <t>Blue</t>
   </si>
   <si>
-    <t>CHIPLED_0603</t>
-  </si>
-  <si>
     <t>OVS-0603</t>
   </si>
   <si>
-    <t>CHIP-LED0603</t>
-  </si>
-  <si>
     <t>OVS-0604</t>
   </si>
   <si>
     <t>31k6</t>
   </si>
   <si>
-    <t>R0603</t>
-  </si>
-  <si>
     <t>MC0063W060311K5</t>
   </si>
   <si>
@@ -144,9 +114,6 @@
     <t>LT3686HDDPBF</t>
   </si>
   <si>
-    <t>DFN300X300X80-11N</t>
-  </si>
-  <si>
     <t>LT3686HDD#PBF</t>
   </si>
   <si>
@@ -201,37 +168,19 @@
     <t>Qty</t>
   </si>
   <si>
-    <t>Device</t>
-  </si>
-  <si>
     <t>Parts</t>
   </si>
   <si>
     <t>MPN</t>
   </si>
   <si>
-    <t>C-EUC0603</t>
-  </si>
-  <si>
-    <t>R-EU_R0603</t>
-  </si>
-  <si>
     <t>CONNECTOR</t>
   </si>
   <si>
-    <t>C-EUC0805</t>
-  </si>
-  <si>
     <t>MCMT21N220F250CT</t>
   </si>
   <si>
-    <t>LEDCHIP-LED0603</t>
-  </si>
-  <si>
     <t>LED</t>
-  </si>
-  <si>
-    <t>LEDCHIPLED_0603</t>
   </si>
   <si>
     <t>Fuse</t>
@@ -447,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -463,9 +412,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -499,7 +445,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="10">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -507,44 +453,6 @@
           <color indexed="64"/>
         </left>
         <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -763,16 +671,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:G19" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="A1:G19"/>
-  <sortState ref="A2:G19">
-    <sortCondition ref="E1:E19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E19" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="A1:E19"/>
+  <sortState ref="A2:E19">
+    <sortCondition ref="C1:C19"/>
   </sortState>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Qty" dataDxfId="6"/>
-    <tableColumn id="2" name="Value" dataDxfId="5"/>
-    <tableColumn id="3" name="Device" dataDxfId="4"/>
-    <tableColumn id="4" name="Package" dataDxfId="3"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Qty" dataDxfId="4"/>
+    <tableColumn id="2" name="Value" dataDxfId="3"/>
     <tableColumn id="5" name="Parts" dataDxfId="2"/>
     <tableColumn id="6" name="Description" dataDxfId="1"/>
     <tableColumn id="7" name="MPN" dataDxfId="0"/>
@@ -1092,51 +998,51 @@
   <sheetData>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B10" s="3">
         <f ca="1">TODAY()</f>
-        <v>42760</v>
+        <v>42776</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1150,474 +1056,359 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="64.140625" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" customWidth="1"/>
-    <col min="11" max="12" width="17.140625" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" customWidth="1"/>
-    <col min="14" max="14" width="10" customWidth="1"/>
-    <col min="15" max="15" width="7.42578125" customWidth="1"/>
-    <col min="16" max="16" width="6.42578125" customWidth="1"/>
-    <col min="17" max="17" width="11.140625" customWidth="1"/>
-    <col min="18" max="18" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="64.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" customWidth="1"/>
+    <col min="9" max="10" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" customWidth="1"/>
+    <col min="12" max="12" width="10" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" customWidth="1"/>
+    <col min="14" max="14" width="6.42578125" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>57</v>
+      <c r="C1" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="12" t="s">
+      <c r="E1" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>2</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" s="9" t="s">
+      <c r="C3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G3" s="9" t="s">
+      <c r="C4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="C5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="C6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>1</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="C7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="8">
+        <v>3557</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="C8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="8">
+        <v>74477410</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="8">
+        <v>744774115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>2</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="E11" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
         <v>2</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>1</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" s="9">
-        <v>3557</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>2</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="7">
-        <v>2007041</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
-        <v>1</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G9" s="9">
-        <v>74477410</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
-        <v>1</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G10" s="9">
-        <v>744774115</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
-        <v>2</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <v>2</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>3</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>2</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>1</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>2</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12" s="9" t="s">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>4</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
-        <v>3</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="C17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>2</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="C18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <v>2</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
         <v>1</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>2</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <v>4</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G17" s="9" t="s">
+      <c r="B19" s="14" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
-        <v>2</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
-        <v>1</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="G19" s="16">
+      <c r="C19" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="15">
         <v>1757242</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="68" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="91" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>